<commit_message>
Updated the battery on the BOM to the correct one
</commit_message>
<xml_diff>
--- a/Version WIP/Aegis 2 BOM.xlsx
+++ b/Version WIP/Aegis 2 BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jucke\Dropbox\Projects\Aegis 2\Aegis-2\Version 1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jucke\Dropbox\Projects\Aegis 2\Aegis-2\Version WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F79DA6-6080-4D51-A44A-CDE393A19F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A81F0E-BACE-4DD5-BF1A-5DEEBA43C0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{93BD1906-D6D6-45EE-A20C-B1437B097662}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{93BD1906-D6D6-45EE-A20C-B1437B097662}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board" sheetId="1" r:id="rId1"/>
@@ -375,9 +375,6 @@
     <t>https://www.digikey.com/en/products/detail/assmann-wsw-components/V5618A/3511413</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32909360073.html?spm=a2g0o.detail.1000060.1.e7e11d8fuRaTNk&amp;gps-id=pcDetailBottomMoreThisSeller&amp;scm=1007.13339.169870.0&amp;scm_id=1007.13339.169870.0&amp;scm-url=1007.13339.169870.0&amp;pvid=26070229-41e1-4524-b5d5-b93a95b1a8fc&amp;_t=gps-id:pcDetailBottomMoreThisSeller,scm-url:1007.13339.169870.0,pvid:26070229-41e1-4524-b5d5-b93a95b1a8fc,tpp_buckets:668%230%23131923%2312_668%23808%234094%23798_668%23888%233325%238_668%234328%2319925%23153_668%232846%238112%23594_668%232717%237567%23903_668%231000022185%231000066058%230_668%233468%2315608%23141</t>
-  </si>
-  <si>
     <t>Teensy Header</t>
   </si>
   <si>
@@ -985,6 +982,9 @@
   </si>
   <si>
     <t>BUTTONS</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256802895965671.html?spm=a2g0o.order_list.order_list_main.111.675d1802dWILfE&amp;gatewayAdapt=glo2usa4itemAdapt</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1061,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1092,12 +1092,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1458,7 +1452,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1467,7 +1461,7 @@
         <v>4.54</v>
       </c>
       <c r="E3" s="4">
-        <f>D3*C3</f>
+        <f t="shared" ref="E3:E11" si="0">D3*C3</f>
         <v>4.54</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1479,7 +1473,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1488,7 +1482,7 @@
         <v>3.04</v>
       </c>
       <c r="E4" s="4">
-        <f>D4*C4</f>
+        <f t="shared" si="0"/>
         <v>3.04</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1497,10 +1491,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1509,19 +1503,19 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="E5" s="4">
-        <f>D5*C5</f>
+        <f t="shared" si="0"/>
         <v>2.4300000000000002</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1530,19 +1524,19 @@
         <v>3.37</v>
       </c>
       <c r="E6" s="4">
-        <f>D6*C6</f>
+        <f t="shared" si="0"/>
         <v>3.37</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>218</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1551,19 +1545,19 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="4">
-        <f>D7*C7</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1572,19 +1566,19 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="4">
-        <f>D8*C8</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1593,19 +1587,19 @@
         <v>0.93</v>
       </c>
       <c r="E9" s="4">
-        <f>D9*C9</f>
+        <f t="shared" si="0"/>
         <v>1.86</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>226</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>227</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1614,19 +1608,19 @@
         <v>0.7</v>
       </c>
       <c r="E10" s="4">
-        <f>D10*C10</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1635,11 +1629,11 @@
         <v>6.04</v>
       </c>
       <c r="E11" s="4">
-        <f>D11*C11</f>
+        <f t="shared" si="0"/>
         <v>6.04</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1656,7 +1650,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1683,7 +1677,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1696,7 +1690,7 @@
         <v>3.8</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1704,7 +1698,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1713,7 +1707,7 @@
         <v>3.87</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" ref="E18:E21" si="0">D18*C18</f>
+        <f t="shared" ref="E18:E21" si="1">D18*C18</f>
         <v>3.87</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -1725,7 +1719,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1734,7 +1728,7 @@
         <v>0.46</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.46</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1746,7 +1740,7 @@
         <v>47</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1755,7 +1749,7 @@
         <v>0.59</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -1764,10 +1758,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1776,11 +1770,11 @@
         <v>0.8</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1794,7 +1788,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1807,7 +1801,7 @@
         <v>1.94</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1815,7 +1809,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1842,7 +1836,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1855,15 +1849,15 @@
         <v>3</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1876,7 +1870,7 @@
         <v>0.92</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1884,15 +1878,15 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>213</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1905,7 +1899,7 @@
         <v>1.38</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1922,7 +1916,7 @@
         <v>62</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1940,10 +1934,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1956,7 +1950,7 @@
         <v>4.03</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1973,7 +1967,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -1982,7 +1976,7 @@
         <v>1.77</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" ref="E39:E40" si="1">D39*C39</f>
+        <f t="shared" ref="E39:E40" si="2">D39*C39</f>
         <v>3.54</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -1991,10 +1985,10 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2003,11 +1997,11 @@
         <v>2.12</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.12</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2025,7 +2019,7 @@
         <v>86</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2056,7 +2050,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2085,10 +2079,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2097,11 +2091,11 @@
         <v>0.94</v>
       </c>
       <c r="E49" s="4">
-        <f>D49*C49</f>
+        <f t="shared" ref="E49:E59" si="3">D49*C49</f>
         <v>0.94</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2109,7 +2103,7 @@
         <v>90</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2118,7 +2112,7 @@
         <v>0.11</v>
       </c>
       <c r="E50" s="4">
-        <f>D50*C50</f>
+        <f t="shared" si="3"/>
         <v>0.11</v>
       </c>
       <c r="F50" s="5" t="s">
@@ -2130,7 +2124,7 @@
         <v>76</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -2139,7 +2133,7 @@
         <v>0.18</v>
       </c>
       <c r="E51" s="4">
-        <f>D51*C51</f>
+        <f t="shared" si="3"/>
         <v>0.36</v>
       </c>
       <c r="F51" s="5" t="s">
@@ -2151,7 +2145,7 @@
         <v>77</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2160,7 +2154,7 @@
         <v>0.1</v>
       </c>
       <c r="E52" s="4">
-        <f>D52*C52</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F52" s="5" t="s">
@@ -2172,7 +2166,7 @@
         <v>75</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C53">
         <v>10</v>
@@ -2181,7 +2175,7 @@
         <v>0.1</v>
       </c>
       <c r="E53" s="4">
-        <f>D53*C53</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F53" s="5" t="s">
@@ -2193,7 +2187,7 @@
         <v>93</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -2202,7 +2196,7 @@
         <v>0.11</v>
       </c>
       <c r="E54" s="4">
-        <f>D54*C54</f>
+        <f t="shared" si="3"/>
         <v>0.22</v>
       </c>
       <c r="F54" s="5" t="s">
@@ -2214,7 +2208,7 @@
         <v>94</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2223,7 +2217,7 @@
         <v>0.1</v>
       </c>
       <c r="E55" s="4">
-        <f>D55*C55</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F55" s="5" t="s">
@@ -2232,10 +2226,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C56">
         <v>4</v>
@@ -2244,11 +2238,11 @@
         <v>0.1</v>
       </c>
       <c r="E56" s="4">
-        <f>D56*C56</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2256,7 +2250,7 @@
         <v>84</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2265,7 +2259,7 @@
         <v>0.1</v>
       </c>
       <c r="E57" s="4">
-        <f>D57*C57</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F57" s="5" t="s">
@@ -2274,10 +2268,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2286,7 +2280,7 @@
         <v>0.1</v>
       </c>
       <c r="E58" s="4">
-        <f>D58*C58</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F58" s="5" t="s">
@@ -2298,7 +2292,7 @@
         <v>92</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2307,7 +2301,7 @@
         <v>0.1</v>
       </c>
       <c r="E59" s="4">
-        <f>D59*C59</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F59" s="5" t="s">
@@ -2328,10 +2322,10 @@
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -2344,15 +2338,15 @@
         <v>0.2</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -2361,19 +2355,19 @@
         <v>0.1</v>
       </c>
       <c r="E63" s="4">
-        <f t="shared" ref="E63" si="2">D63*C63</f>
+        <f t="shared" ref="E63" si="4">D63*C63</f>
         <v>0.1</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -2382,11 +2376,11 @@
         <v>0.1</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" ref="E64" si="3">D64*C64</f>
+        <f t="shared" ref="E64" si="5">D64*C64</f>
         <v>0.1</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2394,7 +2388,7 @@
         <v>73</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2403,7 +2397,7 @@
         <v>0.26</v>
       </c>
       <c r="E65" s="4">
-        <f>D65*C65</f>
+        <f t="shared" ref="E65:E75" si="6">D65*C65</f>
         <v>0.26</v>
       </c>
       <c r="F65" s="5" t="s">
@@ -2415,7 +2409,7 @@
         <v>72</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C66">
         <v>7</v>
@@ -2424,19 +2418,19 @@
         <v>0.1</v>
       </c>
       <c r="E66" s="4">
-        <f>D66*C66</f>
+        <f t="shared" si="6"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -2445,19 +2439,19 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E67" s="4">
-        <f>D67*C67</f>
+        <f t="shared" si="6"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -2466,11 +2460,11 @@
         <v>0.11</v>
       </c>
       <c r="E68" s="4">
-        <f>D68*C68</f>
+        <f t="shared" si="6"/>
         <v>0.11</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2478,7 +2472,7 @@
         <v>71</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C69">
         <v>4</v>
@@ -2487,7 +2481,7 @@
         <v>0.27</v>
       </c>
       <c r="E69" s="4">
-        <f>D69*C69</f>
+        <f t="shared" si="6"/>
         <v>1.08</v>
       </c>
       <c r="F69" s="5" t="s">
@@ -2499,7 +2493,7 @@
         <v>80</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -2508,7 +2502,7 @@
         <v>0.13</v>
       </c>
       <c r="E70" s="4">
-        <f>D70*C70</f>
+        <f t="shared" si="6"/>
         <v>0.13</v>
       </c>
       <c r="F70" s="5" t="s">
@@ -2520,7 +2514,7 @@
         <v>74</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2529,11 +2523,11 @@
         <v>0.12</v>
       </c>
       <c r="E71" s="4">
-        <f>D71*C71</f>
+        <f t="shared" si="6"/>
         <v>0.12</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2541,7 +2535,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C72">
         <v>10</v>
@@ -2550,7 +2544,7 @@
         <v>0.18</v>
       </c>
       <c r="E72" s="4">
-        <f>D72*C72</f>
+        <f t="shared" si="6"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="F72" s="5" t="s">
@@ -2562,7 +2556,7 @@
         <v>95</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2571,11 +2565,11 @@
         <v>0.76</v>
       </c>
       <c r="E73" s="4">
-        <f>D73*C73</f>
+        <f t="shared" si="6"/>
         <v>0.76</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2583,7 +2577,7 @@
         <v>81</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2592,19 +2586,19 @@
         <v>0.89</v>
       </c>
       <c r="E74" s="4">
-        <f>D74*C74</f>
+        <f t="shared" si="6"/>
         <v>0.89</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -2613,11 +2607,11 @@
         <v>0.99</v>
       </c>
       <c r="E75" s="4">
-        <f>D75*C75</f>
+        <f t="shared" si="6"/>
         <v>0.99</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2672,7 +2666,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2685,7 +2679,7 @@
         <v>0.37</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2824,10 +2818,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2845,10 +2839,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2861,15 +2855,15 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2881,8 +2875,8 @@
         <f>D5*C5</f>
         <v>0.91</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>255</v>
+      <c r="F5" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2890,16 +2884,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" t="s">
         <v>244</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>245</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2912,15 +2906,15 @@
         <v>0.68</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2933,15 +2927,15 @@
         <v>2.92</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="A10" t="s">
         <v>247</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2954,15 +2948,15 @@
         <v>1.75</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>258</v>
+      <c r="A11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2975,15 +2969,15 @@
         <v>0.39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>259</v>
+      <c r="A12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2996,24 +2990,23 @@
         <v>0.39</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" t="s">
+        <v>269</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3026,12 +3019,11 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -3044,7 +3036,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -3061,11 +3053,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>279</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3078,7 +3070,7 @@
         <v>1.7</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3089,10 +3081,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3105,7 +3097,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3113,7 +3105,7 @@
         <v>43</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3143,7 +3135,7 @@
         <v>86</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3174,7 +3166,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3206,7 +3198,7 @@
         <v>92</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3227,7 +3219,7 @@
         <v>76</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -3245,10 +3237,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3261,7 +3253,7 @@
         <v>0.1</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3269,7 +3261,7 @@
         <v>75</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C35">
         <v>10</v>
@@ -3290,7 +3282,7 @@
         <v>85</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -3311,7 +3303,7 @@
         <v>88</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -3344,7 +3336,7 @@
         <v>87</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -3357,7 +3349,7 @@
         <v>0.4</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3365,7 +3357,7 @@
         <v>72</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -3378,7 +3370,7 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3386,7 +3378,7 @@
         <v>71</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C42">
         <v>11</v>
@@ -3407,7 +3399,7 @@
         <v>80</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3428,7 +3420,7 @@
         <v>70</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -3446,10 +3438,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -3462,7 +3454,7 @@
         <v>0.96</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3475,7 +3467,7 @@
         <v>89</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -3598,16 +3590,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>300</v>
+        <v>243</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3620,15 +3612,15 @@
         <v>0.68</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" t="s">
         <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3641,15 +3633,15 @@
         <v>1.75</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>298</v>
+      <c r="A5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3662,15 +3654,15 @@
         <v>0.39</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>299</v>
+      <c r="A6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>298</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3683,24 +3675,23 @@
         <v>0.39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>270</v>
+      <c r="A9" t="s">
+        <v>269</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3713,12 +3704,11 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3727,11 +3717,11 @@
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>278</v>
+      <c r="A12" t="s">
+        <v>277</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3744,7 +3734,7 @@
         <v>1.7</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3755,10 +3745,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3771,7 +3761,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3779,7 +3769,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3809,7 +3799,7 @@
         <v>86</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3840,7 +3830,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3869,10 +3859,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3885,7 +3875,7 @@
         <v>0.1</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3893,7 +3883,7 @@
         <v>75</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3926,7 +3916,7 @@
         <v>72</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -3939,7 +3929,7 @@
         <v>0.2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3947,7 +3937,7 @@
         <v>70</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -4024,8 +4014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9192E0A5-2D05-4B52-937A-084865A72460}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,10 +4047,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4078,23 +4068,23 @@
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>12.12</v>
+        <v>9.99</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E10" si="0">D3*C3</f>
-        <v>12.12</v>
+        <v>9.99</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>112</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4102,7 +4092,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -4115,15 +4105,15 @@
         <v>7.94</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>131</v>
+      <c r="B5" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -4136,15 +4126,15 @@
         <v>12.95</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4157,7 +4147,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4165,7 +4155,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4177,17 +4167,17 @@
         <f t="shared" si="0"/>
         <v>9.08</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>276</v>
+      <c r="F7" t="s">
+        <v>275</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -4200,7 +4190,7 @@
         <v>8.69</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4208,7 +4198,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -4221,7 +4211,7 @@
         <v>4.34</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4229,7 +4219,7 @@
         <v>110</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -4250,7 +4240,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4268,10 +4258,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>301</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -4284,15 +4274,15 @@
         <v>24.76</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -4305,15 +4295,15 @@
         <v>1.93</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -4326,15 +4316,15 @@
         <v>1.86</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>311</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -4347,15 +4337,15 @@
         <v>13.28</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -4368,7 +4358,7 @@
         <v>13.99</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4378,17 +4368,17 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B18" s="15"/>
+        <v>265</v>
+      </c>
+      <c r="B18" s="7"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>262</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4401,15 +4391,15 @@
         <v>2.68</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>269</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -4422,25 +4412,24 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
+      <c r="B21" s="7"/>
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" s="7"/>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="7"/>
       <c r="D23">
@@ -4450,7 +4439,7 @@
         <v>6.9</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -4462,7 +4451,7 @@
       </c>
       <c r="E25" s="4">
         <f>SUM(E2:E23)</f>
-        <v>178.75000000000003</v>
+        <v>176.62000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: adding new files I never got around to adding.
</commit_message>
<xml_diff>
--- a/Version WIP/Aegis 2 BOM.xlsx
+++ b/Version WIP/Aegis 2 BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jucke\Dropbox\Projects\Aegis 2\Aegis-2\Version WIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djuckett\Dropbox\Projects\Aegis 2\Aegis-2\Version WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A81F0E-BACE-4DD5-BF1A-5DEEBA43C0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E7D823-75A2-479A-810E-653DB9E74DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{93BD1906-D6D6-45EE-A20C-B1437B097662}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{93BD1906-D6D6-45EE-A20C-B1437B097662}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board" sheetId="1" r:id="rId1"/>
@@ -627,9 +627,6 @@
     <t>https://www.digikey.com/en/products/detail/yageo/CC0603KPX7R9BB471/691810</t>
   </si>
   <si>
-    <t>Cap  0.33 uF (603)</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10B334KA8VPNC/11487786</t>
   </si>
   <si>
@@ -642,15 +639,9 @@
     <t>R2</t>
   </si>
   <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>R6, R7, R8, R9, R10, R11, R12, R13, R14, R15</t>
-  </si>
-  <si>
     <t>R16, R17</t>
   </si>
   <si>
@@ -864,9 +855,6 @@
     <t>https://www.amazon.com/Dedicated-Aluminum-Heatsink-Raspberry-Compute/dp/B093FSS6XX/ref=asc_df_B093FSS6XX/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=647248209079&amp;hvpos=&amp;hvnetw=g&amp;hvrand=4581538439163296605&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9016965&amp;hvtargid=pla-2007964195647&amp;gclid=CjwKCAjw3ueiBhBmEiwA4BhspC4oXb-6Z3YZKl8dphxldkEmSZ_R6mIv_rni8NS5jTlwWlrca2spgRoCp7AQAvD_BwE&amp;th=1</t>
   </si>
   <si>
-    <t>Fan is no longer available on Aliepxress, need to look for a new source</t>
-  </si>
-  <si>
     <t>PI_CM4</t>
   </si>
   <si>
@@ -985,6 +973,18 @@
   </si>
   <si>
     <t>https://www.aliexpress.us/item/3256802895965671.html?spm=a2g0o.order_list.order_list_main.111.675d1802dWILfE&amp;gatewayAdapt=glo2usa4itemAdapt</t>
+  </si>
+  <si>
+    <t>Cap  330 nF (603)</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256803228333750.html?spm=a2g0o.productlist.main.1.27357aedfOveIi&amp;algo_pvid=b9289e00-9e59-4056-b51a-43910fcea86f&amp;algo_exp_id=b9289e00-9e59-4056-b51a-43910fcea86f-0&amp;pdp_npi=3%40dis%21USD%2111.59%219.62%21%21%21%21%21%40212278bd16865808440348119d07cd%2112000025683190881%21sea%21US%211888726260&amp;curPageLogUid=DbxWuEx0YQy9</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R3, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15</t>
   </si>
 </sst>
 </file>
@@ -1040,12 +1040,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1061,7 +1067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1092,6 +1098,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1409,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6707F135-86D3-4C44-830B-55C19C13F6FB}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,10 +1540,10 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1549,15 +1556,15 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1570,15 +1577,15 @@
         <v>0.2</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1591,15 +1598,15 @@
         <v>1.86</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1612,15 +1619,15 @@
         <v>0.7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1633,7 +1640,7 @@
         <v>6.04</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1836,7 +1843,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1849,15 +1856,15 @@
         <v>3</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1870,7 +1877,7 @@
         <v>0.92</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1878,15 +1885,15 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1899,7 +1906,7 @@
         <v>1.38</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1985,10 +1992,10 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2001,7 +2008,7 @@
         <v>2.12</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2026,7 @@
         <v>86</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2050,7 +2057,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2082,7 +2089,7 @@
         <v>169</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2103,7 +2110,7 @@
         <v>90</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2124,17 +2131,17 @@
         <v>76</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>201</v>
+        <v>314</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="4">
         <v>0.18</v>
       </c>
       <c r="E51" s="4">
         <f t="shared" si="3"/>
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>104</v>
@@ -2145,7 +2152,7 @@
         <v>77</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2166,17 +2173,17 @@
         <v>75</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>203</v>
+        <v>315</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D53" s="4">
         <v>0.1</v>
       </c>
       <c r="E53" s="4">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>15</v>
@@ -2187,7 +2194,7 @@
         <v>93</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -2208,7 +2215,7 @@
         <v>94</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2229,7 +2236,7 @@
         <v>125</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C56">
         <v>4</v>
@@ -2250,7 +2257,7 @@
         <v>84</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2271,7 +2278,7 @@
         <v>124</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2292,7 +2299,7 @@
         <v>92</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2427,7 +2434,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>196</v>
+        <v>312</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>180</v>
@@ -2443,7 +2450,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2527,7 +2534,7 @@
         <v>0.12</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2700,11 +2707,11 @@
       </c>
       <c r="B83" s="9">
         <f>SUM(E2:E80)</f>
-        <v>67.97999999999999</v>
+        <v>67.899999999999991</v>
       </c>
       <c r="C83" s="4">
         <f>B83/1</f>
-        <v>67.97999999999999</v>
+        <v>67.899999999999991</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2768,9 +2775,14 @@
     <hyperlink ref="F56" r:id="rId39" xr:uid="{CF4C28CD-42DB-410E-93A8-2CA1C27A8C6A}"/>
     <hyperlink ref="F6" r:id="rId40" xr:uid="{88B43D37-ED21-421E-8DE4-4A9BC1856308}"/>
     <hyperlink ref="F32" r:id="rId41" xr:uid="{A168D9F0-C6CE-4665-8C5B-EB1FF16812E5}"/>
+    <hyperlink ref="F7" r:id="rId42" xr:uid="{5A545753-6BAE-4E93-BD3F-7015D416345E}"/>
+    <hyperlink ref="F8" r:id="rId43" xr:uid="{1D57C2C6-69F9-44B1-964A-8806C8F505BE}"/>
+    <hyperlink ref="F9" r:id="rId44" xr:uid="{0FF96674-38C4-43D9-8178-B8612EF4B766}"/>
+    <hyperlink ref="F10" r:id="rId45" xr:uid="{240C0BBB-5F46-443B-8975-6A4001EE6F2C}"/>
+    <hyperlink ref="F11" r:id="rId46" xr:uid="{AD6D1C95-A83C-44FC-B812-7856EDE97CD8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -2778,8 +2790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D53D821-8485-49D1-9F30-5E1E50B18DEC}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,7 +2830,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>141</v>
@@ -2839,10 +2851,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2860,10 +2872,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2876,7 +2888,7 @@
         <v>0.91</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2884,16 +2896,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2906,15 +2918,15 @@
         <v>0.68</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2927,15 +2939,15 @@
         <v>2.92</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2948,15 +2960,15 @@
         <v>1.75</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2969,15 +2981,15 @@
         <v>0.39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2990,7 +3002,7 @@
         <v>0.39</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2998,15 +3010,15 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3019,7 +3031,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3054,10 +3066,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3070,7 +3082,7 @@
         <v>1.7</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,11 +3092,11 @@
       <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="14" t="s">
         <v>159</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3105,7 +3117,7 @@
         <v>43</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3135,7 +3147,7 @@
         <v>86</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3166,7 +3178,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3198,7 +3210,7 @@
         <v>92</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3219,7 +3231,7 @@
         <v>76</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -3240,7 +3252,7 @@
         <v>128</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3261,7 +3273,7 @@
         <v>75</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C35">
         <v>10</v>
@@ -3282,7 +3294,7 @@
         <v>85</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -3303,7 +3315,7 @@
         <v>88</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -3349,7 +3361,7 @@
         <v>0.4</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3357,7 +3369,7 @@
         <v>72</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -3378,7 +3390,7 @@
         <v>71</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C42">
         <v>11</v>
@@ -3399,7 +3411,7 @@
         <v>80</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3420,7 +3432,7 @@
         <v>70</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -3438,10 +3450,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -3467,7 +3479,7 @@
         <v>89</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -3546,9 +3558,10 @@
     <hyperlink ref="F35" r:id="rId19" xr:uid="{0FF516AE-C3FF-4485-9872-2719916BD263}"/>
     <hyperlink ref="F34" r:id="rId20" xr:uid="{311BC1A4-1213-4AD6-93EB-15BA831AC69A}"/>
     <hyperlink ref="F41" r:id="rId21" xr:uid="{469E9AFB-BF8A-49CD-8753-62E512A8B747}"/>
+    <hyperlink ref="F19" r:id="rId22" display="https://www.ebay.com/itm/354618455099?chn=ps&amp;var=623990696410&amp;_trkparms=ispr%3D1&amp;amdata=enc%3A1Zk6c1fiYQTmjnu1i-GLg_w51&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;mkscid=101&amp;itemid=623990696410_354618455099&amp;targetid=1584739238534&amp;device=c&amp;mktype=&amp;googleloc=9016965&amp;poi=&amp;campaignid=15275224983&amp;mkgroupid=131097072938&amp;rlsatarget=pla-1584739238534&amp;abcId=9300697&amp;merchantid=633191918&amp;gclid=CjwKCAjw3ueiBhBmEiwA4BhspPro6b1IzauVdwTaQfRWhvR-m2RbObJTIP_17MVH22aw1EJwAAuf9hoCW1kQAvD_BwE" xr:uid="{FFB58D04-F635-4E08-965C-1F1978413F1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -3557,7 +3570,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3590,16 +3603,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3612,15 +3625,15 @@
         <v>0.68</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3633,15 +3646,15 @@
         <v>1.75</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3654,15 +3667,15 @@
         <v>0.39</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3675,7 +3688,7 @@
         <v>0.39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3683,15 +3696,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3704,7 +3717,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3718,10 +3731,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3734,7 +3747,7 @@
         <v>1.7</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3748,7 +3761,7 @@
         <v>159</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3769,7 +3782,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3799,7 +3812,7 @@
         <v>86</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3830,7 +3843,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3862,7 +3875,7 @@
         <v>128</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3883,7 +3896,7 @@
         <v>75</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -4014,8 +4027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9192E0A5-2D05-4B52-937A-084865A72460}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4084,7 +4097,7 @@
         <v>9.99</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4126,7 +4139,7 @@
         <v>12.95</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4161,20 +4174,20 @@
         <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>9.08</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>9.08</v>
-      </c>
-      <c r="F7" t="s">
-        <v>275</v>
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>313</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>132</v>
@@ -4190,7 +4203,7 @@
         <v>8.69</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4211,7 +4224,7 @@
         <v>4.34</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4240,7 +4253,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -4258,10 +4271,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -4274,15 +4287,15 @@
         <v>24.76</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -4295,15 +4308,15 @@
         <v>1.93</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -4316,15 +4329,15 @@
         <v>1.86</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -4337,15 +4350,15 @@
         <v>13.28</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -4358,7 +4371,7 @@
         <v>13.99</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4368,17 +4381,17 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B18" s="7"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4391,15 +4404,15 @@
         <v>2.68</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -4412,7 +4425,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -4451,7 +4464,7 @@
       </c>
       <c r="E25" s="4">
         <f>SUM(E2:E23)</f>
-        <v>176.62000000000003</v>
+        <v>177.16000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -4673,9 +4686,12 @@
     <hyperlink ref="F2" r:id="rId4" xr:uid="{84970AA0-897C-43E7-B8DF-28D3F3300098}"/>
     <hyperlink ref="F23" r:id="rId5" xr:uid="{216EE6A3-8045-4544-8D98-ABDA82CD9234}"/>
     <hyperlink ref="F10" r:id="rId6" xr:uid="{C96AEF29-4AC2-4257-8AB3-AE09B73FA388}"/>
+    <hyperlink ref="F19" r:id="rId7" xr:uid="{85344F48-5909-4D4E-82AA-60C131CCB21A}"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://www.amazon.com/Dedicated-Aluminum-Heatsink-Raspberry-Compute/dp/B093FSS6XX/ref=asc_df_B093FSS6XX/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=647248209079&amp;hvpos=&amp;hvnetw=g&amp;hvrand=4581538439163296605&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9016965&amp;hvtargid=pla-2007964195647&amp;gclid=CjwKCAjw3ueiBhBmEiwA4BhspC4oXb-6Z3YZKl8dphxldkEmSZ_R6mIv_rni8NS5jTlwWlrca2spgRoCp7AQAvD_BwE&amp;th=1" xr:uid="{4D06C1FE-87B7-4C95-A120-D58694B9DB38}"/>
+    <hyperlink ref="F7" r:id="rId9" display="https://www.aliexpress.us/item/3256803228333750.html?spm=a2g0o.productlist.main.1.27357aedfOveIi&amp;algo_pvid=b9289e00-9e59-4056-b51a-43910fcea86f&amp;algo_exp_id=b9289e00-9e59-4056-b51a-43910fcea86f-0&amp;pdp_npi=3%40dis%21USD%2111.59%219.62%21%21%21%21%21%40212278bd16865808440348119d07cd%2112000025683190881%21sea%21US%211888726260&amp;curPageLogUid=DbxWuEx0YQy9" xr:uid="{5CC8DA23-2F67-4CD0-A0DF-630E6A932E55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>